<commit_message>
ch 7 sec 3 hw problems done
</commit_message>
<xml_diff>
--- a/0_Resources/Problems/7_Power_Query/1_Power_Query_Intro_Problem.xlsx
+++ b/0_Resources/Problems/7_Power_Query/1_Power_Query_Intro_Problem.xlsx
@@ -1,20 +1,19 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28025"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28122"/>
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\SaderPC\Documents\GitHub\Excel_Data_Analytics_Course\0_Resources\Problems\7_Power_Query\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="\\Mac\Home\Developer\_Courses\Excel\Excel_Data_Analytics_Course\0_Resources\Problems\7_Power_Query\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{34C5C7A3-CF20-4BE2-803A-14226DF476CE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="8_{7FC0F96F-DD62-4364-B1CF-9503063349E3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" activeTab="1" xr2:uid="{7E364698-D443-4A94-B95B-7CD99D62E073}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="38620" windowHeight="21820" xr2:uid="{493E9804-432C-452D-9AA0-1068E23E4A49}"/>
   </bookViews>
   <sheets>
-    <sheet name="7-1-1" sheetId="1" r:id="rId1"/>
-    <sheet name="7-1-2" sheetId="2" r:id="rId2"/>
+    <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -402,24 +401,12 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{EE8CC960-B49A-4CA4-8FBD-34077EE849F5}">
-  <dimension ref="A1"/>
-  <sheetViews>
-    <sheetView workbookViewId="0"/>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <sheetData/>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{22586523-C526-47C0-B802-E65CC4EE3A02}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6BE3599E-640C-4122-A7EB-4816C7B00BF1}">
   <dimension ref="A1"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <sheetData/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>